<commit_message>
Add gain linearity graph
</commit_message>
<xml_diff>
--- a/CMCEC Gain Calibration.xlsx
+++ b/CMCEC Gain Calibration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\F3rni\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3143615-D58B-4EB9-B98E-EEFA6B71E555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D960C3B-E970-4FDE-AF14-7883C7D228C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{31551E4A-DA23-44B1-BA5A-014C8EAB6FF5}"/>
   </bookViews>
@@ -488,7 +488,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -500,6 +500,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -507,18 +525,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -539,20 +545,20 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -570,6 +576,974 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Gain</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> linearity</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$7:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$D$7:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.84</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8266666666666669</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.83</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8280000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.83</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8314285714285714</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-717E-41C9-9924-56F17A5DD0DB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="2065443024"/>
+        <c:axId val="2065457584"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="2065443024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2065457584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="2065457584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3"/>
+          <c:min val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2065443024"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>876299</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>607218</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8C10AD4-7B12-4BE1-B496-9F3B80F8AAA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -869,10 +1843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FCE0A18-19CA-41B8-957C-9BD62847CD37}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,59 +1857,66 @@
     <col min="5" max="5" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="20"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="27"/>
     </row>
-    <row r="3" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="13"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
     </row>
-    <row r="4" spans="1:4" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+    <row r="4" spans="1:11" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="16"/>
+      <c r="B4" s="29"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="30"/>
     </row>
-    <row r="5" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="26"/>
-      <c r="B5" s="17" t="s">
+    <row r="5" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="14"/>
+      <c r="B5" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="27" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="16" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="30" t="s">
+      <c r="D6" s="18" t="s">
         <v>0</v>
       </c>
+      <c r="E6" s="32"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="31"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="31"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>0.5</v>
       </c>
@@ -944,11 +1925,18 @@
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="9">
-        <f>B7/A7</f>
+        <f t="shared" ref="D7:D14" si="0">B7/A7</f>
         <v>1.84</v>
       </c>
+      <c r="E7" s="32"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="31"/>
+      <c r="J7" s="31"/>
+      <c r="K7" s="31"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>1</v>
       </c>
@@ -957,11 +1945,18 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="9">
-        <f>B8/A8</f>
+        <f t="shared" si="0"/>
         <v>1.83</v>
       </c>
+      <c r="E8" s="32"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>1.5</v>
       </c>
@@ -970,11 +1965,18 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="9">
-        <f>B9/A9</f>
+        <f t="shared" si="0"/>
         <v>1.8266666666666669</v>
       </c>
+      <c r="E9" s="32"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>2</v>
       </c>
@@ -983,11 +1985,18 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="9">
-        <f>B10/A10</f>
+        <f t="shared" si="0"/>
         <v>1.83</v>
       </c>
+      <c r="E10" s="32"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>2.5</v>
       </c>
@@ -996,11 +2005,18 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="9">
-        <f>B11/A11</f>
+        <f t="shared" si="0"/>
         <v>1.8280000000000001</v>
       </c>
+      <c r="E11" s="32"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
+      <c r="H11" s="31"/>
+      <c r="I11" s="31"/>
+      <c r="J11" s="31"/>
+      <c r="K11" s="31"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>3</v>
       </c>
@@ -1009,11 +2025,18 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="9">
-        <f>B12/A12</f>
+        <f t="shared" si="0"/>
         <v>1.83</v>
       </c>
+      <c r="E12" s="32"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>3.5</v>
       </c>
@@ -1022,11 +2045,18 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="9">
-        <f>B13/A13</f>
+        <f t="shared" si="0"/>
         <v>1.8314285714285714</v>
       </c>
+      <c r="E13" s="32"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>4</v>
       </c>
@@ -1035,25 +2065,46 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="9">
-        <f>B14/A14</f>
+        <f t="shared" si="0"/>
         <v>1.83</v>
       </c>
+      <c r="E14" s="32"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="4"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="31"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="29" t="s">
+      <c r="D16" s="17" t="s">
         <v>5</v>
       </c>
+      <c r="E16" s="32"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="31"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
@@ -1061,18 +2112,27 @@
         <f>AVERAGE(D7:D14)</f>
         <v>1.8307619047619048</v>
       </c>
+      <c r="E17" s="32"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
+      <c r="J17" s="31"/>
+      <c r="K17" s="31"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E6:K17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{E3730376-0FD9-4C09-BD9C-F2A4C9CEF84F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>